<commit_message>
Added all symbiont density sample data
</commit_message>
<xml_diff>
--- a/data/baseline_sampling/sym_counts.xlsx
+++ b/data/baseline_sampling/sym_counts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/apulchra_metabolism/data/baseline_sampling/sym_counts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/apulchra_metabolism/data/baseline_sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBAF33D-9B3D-0643-95A7-15F67230AB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326412D9-FB9C-5F4F-8B73-0F87F0EC32C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="27640" windowHeight="16000" xr2:uid="{3F637B6A-34B6-C147-9B30-DF4A4399AD70}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="27640" windowHeight="16000" xr2:uid="{3F637B6A-34B6-C147-9B30-DF4A4399AD70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>fragment</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>AH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AH, TA </t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4602EE8-CFD7-B245-B048-E3FD6748E901}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,42 +629,96 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="e">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>161</v>
+      </c>
+      <c r="D3">
+        <v>178</v>
+      </c>
+      <c r="E3">
+        <v>182</v>
+      </c>
+      <c r="F3">
+        <v>172</v>
+      </c>
+      <c r="G3">
+        <v>158</v>
+      </c>
+      <c r="H3">
+        <v>185</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3">
         <f t="shared" ref="J3:J26" si="0">AVERAGE(C3:H3)/B3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K3" t="e">
+        <v>86.333333333333329</v>
+      </c>
+      <c r="K3">
         <f t="shared" ref="K3:K26" si="1">STDEV(C3:H3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L3" t="e">
+        <v>11.129540272026812</v>
+      </c>
+      <c r="L3">
         <f t="shared" ref="L3:L26" si="2">(K3/J3)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M3" t="e">
+        <v>12.891359388448045</v>
+      </c>
+      <c r="M3">
         <f t="shared" ref="M3:M26" si="3">J3*(10^4)</f>
-        <v>#DIV/0!</v>
+        <v>863333.33333333326</v>
+      </c>
+      <c r="N3">
+        <v>20221017</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>122</v>
+      </c>
+      <c r="D4">
+        <v>112</v>
+      </c>
+      <c r="E4">
+        <v>120</v>
+      </c>
+      <c r="F4">
+        <v>115</v>
+      </c>
+      <c r="G4">
+        <v>114</v>
+      </c>
+      <c r="H4">
+        <v>130</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>39.611111111111107</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>6.6458006791256281</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>16.777617422757547</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>396111.11111111107</v>
+      </c>
+      <c r="N4">
+        <v>20221017</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -812,21 +869,48 @@
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="J8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>112</v>
+      </c>
+      <c r="D8">
+        <v>118</v>
+      </c>
+      <c r="E8">
+        <v>107</v>
+      </c>
+      <c r="F8">
+        <v>105</v>
+      </c>
+      <c r="G8">
+        <v>105</v>
+      </c>
+      <c r="H8">
+        <v>115</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>36.777777777777779</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>5.5015149428740688</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>14.95880195947632</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>367777.77777777781</v>
+      </c>
+      <c r="N8">
+        <v>20221017</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -929,42 +1013,96 @@
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="J11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L11" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>124</v>
+      </c>
+      <c r="D11">
+        <v>119</v>
+      </c>
+      <c r="E11">
+        <v>113</v>
+      </c>
+      <c r="F11">
+        <v>104</v>
+      </c>
+      <c r="G11">
+        <v>114</v>
+      </c>
+      <c r="H11">
+        <v>107</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>113.5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>7.3959448348402388</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>6.5162509558063784</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>1135000</v>
+      </c>
+      <c r="N11">
+        <v>20221017</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="J12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>218</v>
+      </c>
+      <c r="D12">
+        <v>220</v>
+      </c>
+      <c r="E12">
+        <v>219</v>
+      </c>
+      <c r="F12">
+        <v>228</v>
+      </c>
+      <c r="G12">
+        <v>238</v>
+      </c>
+      <c r="H12">
+        <v>204</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>110.58333333333333</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>11.321071798494463</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>10.237593186279845</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>1105833.3333333333</v>
+      </c>
+      <c r="N12">
+        <v>20221017</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1181,6 +1319,9 @@
       <c r="H17">
         <v>302</v>
       </c>
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
       <c r="J17">
         <f t="shared" si="0"/>
         <v>299.66666666666669</v>
@@ -1205,21 +1346,48 @@
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="J18" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>152</v>
+      </c>
+      <c r="D18">
+        <v>170</v>
+      </c>
+      <c r="E18">
+        <v>161</v>
+      </c>
+      <c r="F18">
+        <v>160</v>
+      </c>
+      <c r="G18">
+        <v>143</v>
+      </c>
+      <c r="H18">
+        <v>150</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>9.5707888912043195</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>6.1351210841053323</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>1560000</v>
+      </c>
+      <c r="N18">
+        <v>20221017</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -1274,42 +1442,96 @@
       <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="J20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>169</v>
+      </c>
+      <c r="D20">
+        <v>165</v>
+      </c>
+      <c r="E20">
+        <v>155</v>
+      </c>
+      <c r="F20">
+        <v>156</v>
+      </c>
+      <c r="G20">
+        <v>159</v>
+      </c>
+      <c r="H20">
+        <v>158</v>
+      </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>40.083333333333336</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>5.5015149428740679</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>13.725193204675429</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>400833.33333333337</v>
+      </c>
+      <c r="N20">
+        <v>20221017</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="J21" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>181</v>
+      </c>
+      <c r="D21">
+        <v>173</v>
+      </c>
+      <c r="E21">
+        <v>205</v>
+      </c>
+      <c r="F21">
+        <v>204</v>
+      </c>
+      <c r="G21">
+        <v>180</v>
+      </c>
+      <c r="H21">
+        <v>174</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>93.083333333333329</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>14.552204873030982</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>15.633523587857814</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>930833.33333333326</v>
+      </c>
+      <c r="N21">
+        <v>20221017</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -1364,81 +1586,144 @@
       <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="J23" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L23" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>179</v>
+      </c>
+      <c r="D23">
+        <v>175</v>
+      </c>
+      <c r="E23">
+        <v>186</v>
+      </c>
+      <c r="F23">
+        <v>207</v>
+      </c>
+      <c r="G23">
+        <v>187</v>
+      </c>
+      <c r="H23">
+        <v>171</v>
+      </c>
+      <c r="I23" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>184.16666666666666</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>12.781497043252275</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>6.9401793900012363</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>1841666.6666666665</v>
+      </c>
+      <c r="N23">
+        <v>20221017</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="J24" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L24" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M24" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>257</v>
+      </c>
+      <c r="D24">
+        <v>232</v>
+      </c>
+      <c r="E24">
+        <v>256</v>
+      </c>
+      <c r="F24">
+        <v>217</v>
+      </c>
+      <c r="G24">
+        <v>250</v>
+      </c>
+      <c r="H24">
+        <v>237</v>
+      </c>
+      <c r="I24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>241.5</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>15.706686474237651</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>6.5038039230797731</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>2415000</v>
+      </c>
+      <c r="N24">
+        <v>20221017</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="J25" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K25" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L25" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J26" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L26" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>118</v>
+      </c>
+      <c r="D25">
+        <v>106</v>
+      </c>
+      <c r="E25">
+        <v>142</v>
+      </c>
+      <c r="F25">
+        <v>114</v>
+      </c>
+      <c r="G25">
+        <v>131</v>
+      </c>
+      <c r="H25">
+        <v>132</v>
+      </c>
+      <c r="I25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>123.83333333333333</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>13.39278412678509</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>10.815168877619184</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>1238333.3333333333</v>
+      </c>
+      <c r="N25">
+        <v>20221017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>